<commit_message>
update se categories, add new acs5 variable files
</commit_message>
<xml_diff>
--- a/src/patterns/acs5_variable_sheets/disability_insurance_grandparents.xlsx
+++ b/src/patterns/acs5_variable_sheets/disability_insurance_grandparents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rwalls/gh/srpdio/src/patterns/acs5_variable_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02594D7C-4213-E34D-8813-10A724A9B308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBD0F44-37E6-FE49-B147-41198B4A3E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="960" windowWidth="27640" windowHeight="16940" xr2:uid="{0FFAD3DD-2A23-3D4E-8E78-846F5FA7885E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="133">
   <si>
     <t>Variable ID</t>
   </si>
@@ -401,13 +401,37 @@
   </si>
   <si>
     <t>age category</t>
+  </si>
+  <si>
+    <t>under 19 years</t>
+  </si>
+  <si>
+    <t>with a disability/with any disability</t>
+  </si>
+  <si>
+    <t>no disability</t>
+  </si>
+  <si>
+    <t>health insurance coverage</t>
+  </si>
+  <si>
+    <t>with health insurance coverage</t>
+  </si>
+  <si>
+    <t>no health insurance coverage</t>
+  </si>
+  <si>
+    <t>with private health insurance coverage</t>
+  </si>
+  <si>
+    <t>with public health coverage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -442,6 +466,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -463,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -479,6 +511,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A539AE3-C618-ED4A-B51A-0222A34BA3AE}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33:O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,12 +844,13 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="8" max="9" width="15.6640625" style="7" customWidth="1"/>
     <col min="10" max="10" width="13.5" style="7" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="7" customWidth="1"/>
     <col min="12" max="12" width="17" style="7" customWidth="1"/>
-    <col min="14" max="14" width="15" style="7" customWidth="1"/>
+    <col min="13" max="14" width="15" style="7" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,17 +881,23 @@
       <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>123</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="N1" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O1" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -882,10 +924,16 @@
         <v>124</v>
       </c>
       <c r="J2" s="6"/>
+      <c r="K2" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="L2" s="6"/>
+      <c r="M2" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -910,12 +958,20 @@
       <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="L3" s="6"/>
+      <c r="M3" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -940,14 +996,22 @@
       <c r="H4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J4" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K4" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L4" s="6"/>
+      <c r="M4" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -972,16 +1036,24 @@
       <c r="H5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J5" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K5" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L5" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M5" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1006,18 +1078,29 @@
       <c r="H6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J6" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K6" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L6" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M6" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N6" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O6" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1042,18 +1125,29 @@
       <c r="H7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J7" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K7" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L7" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M7" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N7" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O7" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -1078,16 +1172,24 @@
       <c r="H8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J8" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K8" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L8" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="M8" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
@@ -1112,14 +1214,22 @@
       <c r="H9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J9" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K9" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L9" s="6"/>
+      <c r="M9" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -1144,16 +1254,24 @@
       <c r="H10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J10" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K10" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L10" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M10" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -1178,18 +1296,29 @@
       <c r="H11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J11" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K11" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L11" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M11" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N11" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O11" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -1214,18 +1343,29 @@
       <c r="H12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J12" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K12" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L12" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M12" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N12" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O12" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
@@ -1250,16 +1390,24 @@
       <c r="H13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="J13" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K13" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L13" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="M13" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
@@ -1284,12 +1432,20 @@
       <c r="H14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J14" s="6"/>
+      <c r="K14" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="L14" s="6"/>
+      <c r="M14" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
@@ -1314,14 +1470,22 @@
       <c r="H15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J15" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K15" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L15" s="6"/>
+      <c r="M15" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
@@ -1346,16 +1510,24 @@
       <c r="H16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J16" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K16" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L16" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M16" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="57" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>54</v>
       </c>
@@ -1380,18 +1552,29 @@
       <c r="H17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J17" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K17" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L17" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M17" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N17" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O17" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
@@ -1416,18 +1599,29 @@
       <c r="H18" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J18" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K18" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L18" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M18" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N18" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O18" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -1452,16 +1646,24 @@
       <c r="H19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J19" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K19" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L19" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="M19" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>60</v>
       </c>
@@ -1486,14 +1688,22 @@
       <c r="H20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J20" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K20" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L20" s="6"/>
+      <c r="M20" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N20" s="6"/>
     </row>
-    <row r="21" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -1518,16 +1728,24 @@
       <c r="H21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J21" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K21" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L21" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M21" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="57" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>64</v>
       </c>
@@ -1552,18 +1770,29 @@
       <c r="H22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J22" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K22" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L22" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M22" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N22" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O22" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
@@ -1588,18 +1817,29 @@
       <c r="H23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J23" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K23" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L23" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M23" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N23" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O23" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>68</v>
       </c>
@@ -1624,16 +1864,24 @@
       <c r="H24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J24" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K24" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L24" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="M24" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
@@ -1658,12 +1906,20 @@
       <c r="H25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J25" s="6"/>
+      <c r="K25" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="L25" s="6"/>
+      <c r="M25" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>73</v>
       </c>
@@ -1688,14 +1944,22 @@
       <c r="H26" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I26" s="6"/>
+      <c r="I26" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J26" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K26" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L26" s="6"/>
+      <c r="M26" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>75</v>
       </c>
@@ -1720,16 +1984,24 @@
       <c r="H27" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I27" s="6"/>
+      <c r="I27" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J27" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K27" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L27" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M27" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N27" s="6"/>
     </row>
-    <row r="28" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="57" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>77</v>
       </c>
@@ -1754,18 +2026,29 @@
       <c r="H28" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I28" s="6"/>
+      <c r="I28" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J28" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K28" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L28" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M28" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N28" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O28" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>79</v>
       </c>
@@ -1790,18 +2073,29 @@
       <c r="H29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I29" s="6"/>
+      <c r="I29" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J29" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K29" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L29" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M29" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N29" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O29" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
@@ -1826,16 +2120,24 @@
       <c r="H30" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I30" s="6"/>
+      <c r="I30" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J30" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K30" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="L30" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="M30" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>83</v>
       </c>
@@ -1860,14 +2162,22 @@
       <c r="H31" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I31" s="6"/>
+      <c r="I31" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J31" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K31" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L31" s="6"/>
+      <c r="M31" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>85</v>
       </c>
@@ -1892,16 +2202,24 @@
       <c r="H32" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J32" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K32" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L32" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M32" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="57" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>87</v>
       </c>
@@ -1926,18 +2244,29 @@
       <c r="H33" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J33" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K33" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L33" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M33" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N33" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O33" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>89</v>
       </c>
@@ -1962,18 +2291,29 @@
       <c r="H34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I34" s="6"/>
+      <c r="I34" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J34" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K34" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L34" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M34" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="N34" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="43" x14ac:dyDescent="0.2">
+      <c r="O34" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>91</v>
       </c>
@@ -1998,12 +2338,20 @@
       <c r="H35" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I35" s="6"/>
+      <c r="I35" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="J35" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="K35" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="L35" s="6" t="s">
         <v>35</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="N35" s="6"/>
     </row>

</xml_diff>